<commit_message>
created el salvador page
</commit_message>
<xml_diff>
--- a/visas-centroamerica.xlsx
+++ b/visas-centroamerica.xlsx
@@ -1644,8 +1644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F203"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1653,9 +1653,10 @@
     <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -3330,20 +3331,20 @@
       <c r="B73" t="s">
         <v>155</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>9</v>
+      <c r="C73" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
created costa rica page and made changes in other pages
</commit_message>
<xml_diff>
--- a/visas-centroamerica.xlsx
+++ b/visas-centroamerica.xlsx
@@ -191,9 +191,6 @@
     <t>Bielorrusia</t>
   </si>
   <si>
-    <t>http://www.belarus.by/en/travel/travel-visas</t>
-  </si>
-  <si>
     <t>BLZ</t>
   </si>
   <si>
@@ -1290,6 +1287,9 @@
   </si>
   <si>
     <t>Francia</t>
+  </si>
+  <si>
+    <t>http://mfa.gov.by/upload/17.01.11_list_states_eng.pdf</t>
   </si>
 </sst>
 </file>
@@ -1644,15 +1644,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="G73" sqref="G73"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="A201" sqref="A201:XFD201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" customWidth="1"/>
     <col min="7" max="7" width="16.5" customWidth="1"/>
@@ -2159,7 +2160,7 @@
         <v>17</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>17</v>
@@ -2168,15 +2169,15 @@
         <v>9</v>
       </c>
       <c r="H22" t="s">
-        <v>53</v>
+        <v>419</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
         <v>54</v>
-      </c>
-      <c r="B23" t="s">
-        <v>55</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>17</v>
@@ -2196,10 +2197,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
         <v>56</v>
-      </c>
-      <c r="B24" t="s">
-        <v>57</v>
       </c>
       <c r="C24" t="s">
         <v>24</v>
@@ -2219,10 +2220,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
         <v>58</v>
-      </c>
-      <c r="B25" t="s">
-        <v>59</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>17</v>
@@ -2242,36 +2243,36 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
         <v>60</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" t="s">
         <v>61</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H26" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" t="s">
         <v>63</v>
-      </c>
-      <c r="B27" t="s">
-        <v>64</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>9</v>
@@ -2291,10 +2292,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" t="s">
         <v>65</v>
-      </c>
-      <c r="B28" t="s">
-        <v>66</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>9</v>
@@ -2314,10 +2315,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" t="s">
         <v>67</v>
-      </c>
-      <c r="B29" t="s">
-        <v>68</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>9</v>
@@ -2337,10 +2338,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" t="s">
         <v>69</v>
-      </c>
-      <c r="B30" t="s">
-        <v>70</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>9</v>
@@ -2360,10 +2361,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" t="s">
         <v>71</v>
-      </c>
-      <c r="B31" t="s">
-        <v>72</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>9</v>
@@ -2383,10 +2384,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" t="s">
         <v>73</v>
-      </c>
-      <c r="B32" t="s">
-        <v>74</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>17</v>
@@ -2406,10 +2407,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" t="s">
         <v>75</v>
-      </c>
-      <c r="B33" t="s">
-        <v>76</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>17</v>
@@ -2429,10 +2430,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" t="s">
         <v>77</v>
-      </c>
-      <c r="B34" t="s">
-        <v>78</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>9</v>
@@ -2452,10 +2453,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" t="s">
         <v>79</v>
-      </c>
-      <c r="B35" t="s">
-        <v>80</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>9</v>
@@ -2475,10 +2476,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" t="s">
         <v>81</v>
-      </c>
-      <c r="B36" t="s">
-        <v>82</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>9</v>
@@ -2498,10 +2499,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" t="s">
         <v>83</v>
-      </c>
-      <c r="B37" t="s">
-        <v>84</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>9</v>
@@ -2521,10 +2522,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" t="s">
         <v>85</v>
-      </c>
-      <c r="B38" t="s">
-        <v>86</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>9</v>
@@ -2544,10 +2545,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" t="s">
         <v>87</v>
-      </c>
-      <c r="B39" t="s">
-        <v>88</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>17</v>
@@ -2567,10 +2568,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" t="s">
         <v>89</v>
-      </c>
-      <c r="B40" t="s">
-        <v>90</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>9</v>
@@ -2590,10 +2591,10 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" t="s">
         <v>91</v>
-      </c>
-      <c r="B41" t="s">
-        <v>92</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>9</v>
@@ -2613,10 +2614,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" t="s">
         <v>93</v>
-      </c>
-      <c r="B42" t="s">
-        <v>94</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>17</v>
@@ -2636,10 +2637,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" t="s">
         <v>95</v>
-      </c>
-      <c r="B43" t="s">
-        <v>96</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>9</v>
@@ -2659,10 +2660,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" t="s">
         <v>97</v>
-      </c>
-      <c r="B44" t="s">
-        <v>98</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>17</v>
@@ -2682,10 +2683,10 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>98</v>
+      </c>
+      <c r="B45" t="s">
         <v>99</v>
-      </c>
-      <c r="B45" t="s">
-        <v>100</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>17</v>
@@ -2705,10 +2706,10 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" t="s">
         <v>101</v>
-      </c>
-      <c r="B46" t="s">
-        <v>102</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>17</v>
@@ -2728,10 +2729,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>102</v>
+      </c>
+      <c r="B47" t="s">
         <v>103</v>
-      </c>
-      <c r="B47" t="s">
-        <v>104</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>9</v>
@@ -2751,10 +2752,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>104</v>
+      </c>
+      <c r="B48" t="s">
         <v>105</v>
-      </c>
-      <c r="B48" t="s">
-        <v>106</v>
       </c>
       <c r="C48" t="s">
         <v>24</v>
@@ -2774,10 +2775,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49" t="s">
         <v>107</v>
-      </c>
-      <c r="B49" t="s">
-        <v>108</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>17</v>
@@ -2797,10 +2798,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" t="s">
         <v>109</v>
-      </c>
-      <c r="B50" t="s">
-        <v>110</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>17</v>
@@ -2820,10 +2821,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>110</v>
+      </c>
+      <c r="B51" t="s">
         <v>111</v>
-      </c>
-      <c r="B51" t="s">
-        <v>112</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>9</v>
@@ -2843,10 +2844,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>112</v>
+      </c>
+      <c r="B52" t="s">
         <v>113</v>
-      </c>
-      <c r="B52" t="s">
-        <v>114</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>17</v>
@@ -2866,10 +2867,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>114</v>
+      </c>
+      <c r="B53" t="s">
         <v>115</v>
-      </c>
-      <c r="B53" t="s">
-        <v>116</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>9</v>
@@ -2889,10 +2890,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>116</v>
+      </c>
+      <c r="B54" t="s">
         <v>117</v>
-      </c>
-      <c r="B54" t="s">
-        <v>118</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>9</v>
@@ -2912,10 +2913,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>118</v>
+      </c>
+      <c r="B55" t="s">
         <v>119</v>
-      </c>
-      <c r="B55" t="s">
-        <v>120</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>17</v>
@@ -2935,10 +2936,10 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>120</v>
+      </c>
+      <c r="B56" t="s">
         <v>121</v>
-      </c>
-      <c r="B56" t="s">
-        <v>122</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>17</v>
@@ -2958,10 +2959,10 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>122</v>
+      </c>
+      <c r="B57" t="s">
         <v>123</v>
-      </c>
-      <c r="B57" t="s">
-        <v>124</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>9</v>
@@ -2981,10 +2982,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>124</v>
+      </c>
+      <c r="B58" t="s">
         <v>125</v>
-      </c>
-      <c r="B58" t="s">
-        <v>126</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>17</v>
@@ -3004,10 +3005,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>126</v>
+      </c>
+      <c r="B59" t="s">
         <v>127</v>
-      </c>
-      <c r="B59" t="s">
-        <v>128</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>9</v>
@@ -3027,10 +3028,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B60" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>17</v>
@@ -3050,10 +3051,10 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>129</v>
+      </c>
+      <c r="B61" t="s">
         <v>130</v>
-      </c>
-      <c r="B61" t="s">
-        <v>131</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>17</v>
@@ -3073,10 +3074,10 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>131</v>
+      </c>
+      <c r="B62" t="s">
         <v>132</v>
-      </c>
-      <c r="B62" t="s">
-        <v>133</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>9</v>
@@ -3096,10 +3097,10 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>133</v>
+      </c>
+      <c r="B63" t="s">
         <v>134</v>
-      </c>
-      <c r="B63" t="s">
-        <v>135</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>17</v>
@@ -3119,10 +3120,10 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>135</v>
+      </c>
+      <c r="B64" t="s">
         <v>136</v>
-      </c>
-      <c r="B64" t="s">
-        <v>137</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>9</v>
@@ -3142,10 +3143,10 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>137</v>
+      </c>
+      <c r="B65" t="s">
         <v>138</v>
-      </c>
-      <c r="B65" t="s">
-        <v>139</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>9</v>
@@ -3165,10 +3166,10 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>139</v>
+      </c>
+      <c r="B66" t="s">
         <v>140</v>
-      </c>
-      <c r="B66" t="s">
-        <v>141</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>9</v>
@@ -3188,10 +3189,10 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>141</v>
+      </c>
+      <c r="B67" t="s">
         <v>142</v>
-      </c>
-      <c r="B67" t="s">
-        <v>143</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>9</v>
@@ -3211,10 +3212,10 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>143</v>
+      </c>
+      <c r="B68" t="s">
         <v>144</v>
-      </c>
-      <c r="B68" t="s">
-        <v>145</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>9</v>
@@ -3234,10 +3235,10 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>145</v>
+      </c>
+      <c r="B69" t="s">
         <v>146</v>
-      </c>
-      <c r="B69" t="s">
-        <v>147</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>9</v>
@@ -3257,10 +3258,10 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>147</v>
+      </c>
+      <c r="B70" t="s">
         <v>148</v>
-      </c>
-      <c r="B70" t="s">
-        <v>149</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>17</v>
@@ -3280,10 +3281,10 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>149</v>
+      </c>
+      <c r="B71" t="s">
         <v>150</v>
-      </c>
-      <c r="B71" t="s">
-        <v>151</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>9</v>
@@ -3303,10 +3304,10 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>151</v>
+      </c>
+      <c r="B72" t="s">
         <v>152</v>
-      </c>
-      <c r="B72" t="s">
-        <v>153</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>17</v>
@@ -3326,10 +3327,10 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>153</v>
+      </c>
+      <c r="B73" t="s">
         <v>154</v>
-      </c>
-      <c r="B73" t="s">
-        <v>155</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>17</v>
@@ -3349,10 +3350,10 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>155</v>
+      </c>
+      <c r="B74" t="s">
         <v>156</v>
-      </c>
-      <c r="B74" t="s">
-        <v>157</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>17</v>
@@ -3372,10 +3373,10 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>157</v>
+      </c>
+      <c r="B75" t="s">
         <v>158</v>
-      </c>
-      <c r="B75" t="s">
-        <v>159</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>9</v>
@@ -3395,10 +3396,10 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>159</v>
+      </c>
+      <c r="B76" t="s">
         <v>160</v>
-      </c>
-      <c r="B76" t="s">
-        <v>161</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>9</v>
@@ -3418,10 +3419,10 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>161</v>
+      </c>
+      <c r="B77" t="s">
         <v>162</v>
-      </c>
-      <c r="B77" t="s">
-        <v>163</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>17</v>
@@ -3441,10 +3442,10 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>163</v>
+      </c>
+      <c r="B78" t="s">
         <v>164</v>
-      </c>
-      <c r="B78" t="s">
-        <v>165</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>17</v>
@@ -3464,10 +3465,10 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>165</v>
+      </c>
+      <c r="B79" t="s">
         <v>166</v>
-      </c>
-      <c r="B79" t="s">
-        <v>167</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>17</v>
@@ -3487,10 +3488,10 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>167</v>
+      </c>
+      <c r="B80" t="s">
         <v>168</v>
-      </c>
-      <c r="B80" t="s">
-        <v>169</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>17</v>
@@ -3510,10 +3511,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>169</v>
+      </c>
+      <c r="B81" t="s">
         <v>170</v>
-      </c>
-      <c r="B81" t="s">
-        <v>171</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>9</v>
@@ -3533,10 +3534,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>171</v>
+      </c>
+      <c r="B82" t="s">
         <v>172</v>
-      </c>
-      <c r="B82" t="s">
-        <v>173</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>9</v>
@@ -3556,10 +3557,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>173</v>
+      </c>
+      <c r="B83" t="s">
         <v>174</v>
-      </c>
-      <c r="B83" t="s">
-        <v>175</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>17</v>
@@ -3579,10 +3580,10 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>175</v>
+      </c>
+      <c r="B84" t="s">
         <v>176</v>
-      </c>
-      <c r="B84" t="s">
-        <v>177</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>9</v>
@@ -3602,10 +3603,10 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>177</v>
+      </c>
+      <c r="B85" t="s">
         <v>178</v>
-      </c>
-      <c r="B85" t="s">
-        <v>179</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>9</v>
@@ -3625,10 +3626,10 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>179</v>
+      </c>
+      <c r="B86" t="s">
         <v>180</v>
-      </c>
-      <c r="B86" t="s">
-        <v>181</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>17</v>
@@ -3648,10 +3649,10 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>181</v>
+      </c>
+      <c r="B87" t="s">
         <v>182</v>
-      </c>
-      <c r="B87" t="s">
-        <v>183</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>17</v>
@@ -3671,10 +3672,10 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>183</v>
+      </c>
+      <c r="B88" t="s">
         <v>184</v>
-      </c>
-      <c r="B88" t="s">
-        <v>185</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>17</v>
@@ -3694,10 +3695,10 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>185</v>
+      </c>
+      <c r="B89" t="s">
         <v>186</v>
-      </c>
-      <c r="B89" t="s">
-        <v>187</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>9</v>
@@ -3717,10 +3718,10 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>187</v>
+      </c>
+      <c r="B90" t="s">
         <v>188</v>
-      </c>
-      <c r="B90" t="s">
-        <v>189</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>9</v>
@@ -3740,10 +3741,10 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>189</v>
+      </c>
+      <c r="B91" t="s">
         <v>190</v>
-      </c>
-      <c r="B91" t="s">
-        <v>191</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>17</v>
@@ -3763,10 +3764,10 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>191</v>
+      </c>
+      <c r="B92" t="s">
         <v>192</v>
-      </c>
-      <c r="B92" t="s">
-        <v>193</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>9</v>
@@ -3786,10 +3787,10 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>193</v>
+      </c>
+      <c r="B93" t="s">
         <v>194</v>
-      </c>
-      <c r="B93" t="s">
-        <v>195</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>9</v>
@@ -3809,10 +3810,10 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>195</v>
+      </c>
+      <c r="B94" t="s">
         <v>196</v>
-      </c>
-      <c r="B94" t="s">
-        <v>197</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>9</v>
@@ -3832,10 +3833,10 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>197</v>
+      </c>
+      <c r="B95" t="s">
         <v>198</v>
-      </c>
-      <c r="B95" t="s">
-        <v>199</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>9</v>
@@ -3855,10 +3856,10 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>199</v>
+      </c>
+      <c r="B96" t="s">
         <v>200</v>
-      </c>
-      <c r="B96" t="s">
-        <v>201</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>9</v>
@@ -3878,10 +3879,10 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>201</v>
+      </c>
+      <c r="B97" t="s">
         <v>202</v>
-      </c>
-      <c r="B97" t="s">
-        <v>203</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>9</v>
@@ -3901,10 +3902,10 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>203</v>
+      </c>
+      <c r="B98" t="s">
         <v>204</v>
-      </c>
-      <c r="B98" t="s">
-        <v>205</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>17</v>
@@ -3924,10 +3925,10 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>205</v>
+      </c>
+      <c r="B99" t="s">
         <v>206</v>
-      </c>
-      <c r="B99" t="s">
-        <v>207</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>17</v>
@@ -3947,10 +3948,10 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>207</v>
+      </c>
+      <c r="B100" t="s">
         <v>208</v>
-      </c>
-      <c r="B100" t="s">
-        <v>209</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>17</v>
@@ -3970,10 +3971,10 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
+        <v>209</v>
+      </c>
+      <c r="B101" t="s">
         <v>210</v>
-      </c>
-      <c r="B101" t="s">
-        <v>211</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>9</v>
@@ -3993,10 +3994,10 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>211</v>
+      </c>
+      <c r="B102" t="s">
         <v>212</v>
-      </c>
-      <c r="B102" t="s">
-        <v>213</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>9</v>
@@ -4016,10 +4017,10 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>213</v>
+      </c>
+      <c r="B103" t="s">
         <v>214</v>
-      </c>
-      <c r="B103" t="s">
-        <v>215</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>9</v>
@@ -4039,10 +4040,10 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>215</v>
+      </c>
+      <c r="B104" t="s">
         <v>216</v>
-      </c>
-      <c r="B104" t="s">
-        <v>217</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>9</v>
@@ -4062,10 +4063,10 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>217</v>
+      </c>
+      <c r="B105" t="s">
         <v>218</v>
-      </c>
-      <c r="B105" t="s">
-        <v>219</v>
       </c>
       <c r="C105" t="s">
         <v>24</v>
@@ -4085,10 +4086,10 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>219</v>
+      </c>
+      <c r="B106" t="s">
         <v>220</v>
-      </c>
-      <c r="B106" t="s">
-        <v>221</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>17</v>
@@ -4108,10 +4109,10 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>221</v>
+      </c>
+      <c r="B107" t="s">
         <v>222</v>
-      </c>
-      <c r="B107" t="s">
-        <v>223</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>9</v>
@@ -4131,10 +4132,10 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
+        <v>223</v>
+      </c>
+      <c r="B108" t="s">
         <v>224</v>
-      </c>
-      <c r="B108" t="s">
-        <v>225</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>9</v>
@@ -4154,10 +4155,10 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>225</v>
+      </c>
+      <c r="B109" t="s">
         <v>226</v>
-      </c>
-      <c r="B109" t="s">
-        <v>227</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>17</v>
@@ -4177,10 +4178,10 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>227</v>
+      </c>
+      <c r="B110" t="s">
         <v>228</v>
-      </c>
-      <c r="B110" t="s">
-        <v>229</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>17</v>
@@ -4200,10 +4201,10 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
+        <v>229</v>
+      </c>
+      <c r="B111" t="s">
         <v>230</v>
-      </c>
-      <c r="B111" t="s">
-        <v>231</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>17</v>
@@ -4223,10 +4224,10 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>231</v>
+      </c>
+      <c r="B112" t="s">
         <v>232</v>
-      </c>
-      <c r="B112" t="s">
-        <v>233</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>9</v>
@@ -4246,10 +4247,10 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
+        <v>233</v>
+      </c>
+      <c r="B113" t="s">
         <v>234</v>
-      </c>
-      <c r="B113" t="s">
-        <v>235</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>17</v>
@@ -4269,10 +4270,10 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
+        <v>235</v>
+      </c>
+      <c r="B114" t="s">
         <v>236</v>
-      </c>
-      <c r="B114" t="s">
-        <v>237</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>9</v>
@@ -4292,10 +4293,10 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
+        <v>237</v>
+      </c>
+      <c r="B115" t="s">
         <v>238</v>
-      </c>
-      <c r="B115" t="s">
-        <v>239</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>17</v>
@@ -4315,10 +4316,10 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
+        <v>239</v>
+      </c>
+      <c r="B116" t="s">
         <v>240</v>
-      </c>
-      <c r="B116" t="s">
-        <v>241</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>9</v>
@@ -4338,10 +4339,10 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
+        <v>241</v>
+      </c>
+      <c r="B117" t="s">
         <v>242</v>
-      </c>
-      <c r="B117" t="s">
-        <v>243</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>9</v>
@@ -4361,10 +4362,10 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
+        <v>243</v>
+      </c>
+      <c r="B118" t="s">
         <v>244</v>
-      </c>
-      <c r="B118" t="s">
-        <v>245</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>9</v>
@@ -4384,10 +4385,10 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
+        <v>245</v>
+      </c>
+      <c r="B119" t="s">
         <v>246</v>
-      </c>
-      <c r="B119" t="s">
-        <v>247</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>17</v>
@@ -4407,10 +4408,10 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
+        <v>247</v>
+      </c>
+      <c r="B120" t="s">
         <v>248</v>
-      </c>
-      <c r="B120" t="s">
-        <v>249</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>9</v>
@@ -4430,10 +4431,10 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
+        <v>249</v>
+      </c>
+      <c r="B121" t="s">
         <v>250</v>
-      </c>
-      <c r="B121" t="s">
-        <v>251</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>17</v>
@@ -4453,10 +4454,10 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
+        <v>251</v>
+      </c>
+      <c r="B122" t="s">
         <v>252</v>
-      </c>
-      <c r="B122" t="s">
-        <v>253</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>9</v>
@@ -4476,10 +4477,10 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
+        <v>253</v>
+      </c>
+      <c r="B123" t="s">
         <v>254</v>
-      </c>
-      <c r="B123" t="s">
-        <v>255</v>
       </c>
       <c r="C123" s="4" t="s">
         <v>17</v>
@@ -4499,10 +4500,10 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
+        <v>255</v>
+      </c>
+      <c r="B124" t="s">
         <v>256</v>
-      </c>
-      <c r="B124" t="s">
-        <v>257</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>9</v>
@@ -4522,10 +4523,10 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
+        <v>257</v>
+      </c>
+      <c r="B125" t="s">
         <v>258</v>
-      </c>
-      <c r="B125" t="s">
-        <v>259</v>
       </c>
       <c r="C125" s="2" t="s">
         <v>9</v>
@@ -4545,10 +4546,10 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
+        <v>259</v>
+      </c>
+      <c r="B126" t="s">
         <v>260</v>
-      </c>
-      <c r="B126" t="s">
-        <v>261</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>9</v>
@@ -4568,10 +4569,10 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
+        <v>261</v>
+      </c>
+      <c r="B127" t="s">
         <v>262</v>
-      </c>
-      <c r="B127" t="s">
-        <v>263</v>
       </c>
       <c r="C127" s="2" t="s">
         <v>9</v>
@@ -4591,10 +4592,10 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
+        <v>263</v>
+      </c>
+      <c r="B128" t="s">
         <v>264</v>
-      </c>
-      <c r="B128" t="s">
-        <v>265</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>9</v>
@@ -4614,10 +4615,10 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
+        <v>265</v>
+      </c>
+      <c r="B129" t="s">
         <v>266</v>
-      </c>
-      <c r="B129" t="s">
-        <v>267</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>17</v>
@@ -4637,10 +4638,10 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
+        <v>267</v>
+      </c>
+      <c r="B130" t="s">
         <v>268</v>
-      </c>
-      <c r="B130" t="s">
-        <v>269</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>9</v>
@@ -4660,10 +4661,10 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
+        <v>269</v>
+      </c>
+      <c r="B131" t="s">
         <v>270</v>
-      </c>
-      <c r="B131" t="s">
-        <v>271</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>9</v>
@@ -4683,10 +4684,10 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
+        <v>271</v>
+      </c>
+      <c r="B132" t="s">
         <v>272</v>
-      </c>
-      <c r="B132" t="s">
-        <v>273</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>9</v>
@@ -4706,10 +4707,10 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
+        <v>273</v>
+      </c>
+      <c r="B133" t="s">
         <v>274</v>
-      </c>
-      <c r="B133" t="s">
-        <v>275</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>9</v>
@@ -4729,10 +4730,10 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
+        <v>275</v>
+      </c>
+      <c r="B134" t="s">
         <v>276</v>
-      </c>
-      <c r="B134" t="s">
-        <v>277</v>
       </c>
       <c r="C134" s="4" t="s">
         <v>17</v>
@@ -4752,10 +4753,10 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
+        <v>277</v>
+      </c>
+      <c r="B135" t="s">
         <v>278</v>
-      </c>
-      <c r="B135" t="s">
-        <v>279</v>
       </c>
       <c r="C135" s="4" t="s">
         <v>17</v>
@@ -4775,10 +4776,10 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
+        <v>279</v>
+      </c>
+      <c r="B136" t="s">
         <v>280</v>
-      </c>
-      <c r="B136" t="s">
-        <v>281</v>
       </c>
       <c r="C136" s="4" t="s">
         <v>17</v>
@@ -4798,10 +4799,10 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
+        <v>281</v>
+      </c>
+      <c r="B137" t="s">
         <v>282</v>
-      </c>
-      <c r="B137" t="s">
-        <v>283</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>9</v>
@@ -4821,10 +4822,10 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
+        <v>283</v>
+      </c>
+      <c r="B138" t="s">
         <v>284</v>
-      </c>
-      <c r="B138" t="s">
-        <v>285</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>9</v>
@@ -4844,10 +4845,10 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
+        <v>285</v>
+      </c>
+      <c r="B139" t="s">
         <v>286</v>
-      </c>
-      <c r="B139" t="s">
-        <v>287</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>9</v>
@@ -4867,10 +4868,10 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
+        <v>287</v>
+      </c>
+      <c r="B140" t="s">
         <v>288</v>
-      </c>
-      <c r="B140" t="s">
-        <v>289</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>9</v>
@@ -4890,10 +4891,10 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
+        <v>289</v>
+      </c>
+      <c r="B141" t="s">
         <v>290</v>
-      </c>
-      <c r="B141" t="s">
-        <v>291</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>9</v>
@@ -4913,10 +4914,10 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
+        <v>291</v>
+      </c>
+      <c r="B142" t="s">
         <v>292</v>
-      </c>
-      <c r="B142" t="s">
-        <v>293</v>
       </c>
       <c r="C142" s="4" t="s">
         <v>17</v>
@@ -4936,10 +4937,10 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
+        <v>293</v>
+      </c>
+      <c r="B143" t="s">
         <v>294</v>
-      </c>
-      <c r="B143" t="s">
-        <v>295</v>
       </c>
       <c r="C143" s="2" t="s">
         <v>9</v>
@@ -4959,10 +4960,10 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
+        <v>295</v>
+      </c>
+      <c r="B144" t="s">
         <v>296</v>
-      </c>
-      <c r="B144" t="s">
-        <v>297</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>9</v>
@@ -4982,10 +4983,10 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
+        <v>297</v>
+      </c>
+      <c r="B145" t="s">
         <v>298</v>
-      </c>
-      <c r="B145" t="s">
-        <v>299</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>9</v>
@@ -5005,10 +5006,10 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
+        <v>299</v>
+      </c>
+      <c r="B146" t="s">
         <v>300</v>
-      </c>
-      <c r="B146" t="s">
-        <v>301</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>9</v>
@@ -5028,10 +5029,10 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
+        <v>301</v>
+      </c>
+      <c r="B147" t="s">
         <v>302</v>
-      </c>
-      <c r="B147" t="s">
-        <v>303</v>
       </c>
       <c r="C147" s="4" t="s">
         <v>17</v>
@@ -5051,10 +5052,10 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
+        <v>303</v>
+      </c>
+      <c r="B148" t="s">
         <v>304</v>
-      </c>
-      <c r="B148" t="s">
-        <v>305</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>9</v>
@@ -5074,10 +5075,10 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
+        <v>305</v>
+      </c>
+      <c r="B149" t="s">
         <v>306</v>
-      </c>
-      <c r="B149" t="s">
-        <v>307</v>
       </c>
       <c r="C149" s="4" t="s">
         <v>17</v>
@@ -5097,10 +5098,10 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
+        <v>307</v>
+      </c>
+      <c r="B150" t="s">
         <v>308</v>
-      </c>
-      <c r="B150" t="s">
-        <v>309</v>
       </c>
       <c r="C150" s="4" t="s">
         <v>17</v>
@@ -5120,10 +5121,10 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
+        <v>309</v>
+      </c>
+      <c r="B151" t="s">
         <v>310</v>
-      </c>
-      <c r="B151" t="s">
-        <v>311</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>9</v>
@@ -5143,10 +5144,10 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
+        <v>311</v>
+      </c>
+      <c r="B152" t="s">
         <v>312</v>
-      </c>
-      <c r="B152" t="s">
-        <v>313</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>9</v>
@@ -5166,10 +5167,10 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
+        <v>313</v>
+      </c>
+      <c r="B153" t="s">
         <v>314</v>
-      </c>
-      <c r="B153" t="s">
-        <v>315</v>
       </c>
       <c r="C153" s="4" t="s">
         <v>17</v>
@@ -5189,10 +5190,10 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
+        <v>315</v>
+      </c>
+      <c r="B154" t="s">
         <v>316</v>
-      </c>
-      <c r="B154" t="s">
-        <v>317</v>
       </c>
       <c r="C154" s="4" t="s">
         <v>17</v>
@@ -5212,10 +5213,10 @@
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
+        <v>317</v>
+      </c>
+      <c r="B155" t="s">
         <v>318</v>
-      </c>
-      <c r="B155" t="s">
-        <v>319</v>
       </c>
       <c r="C155" s="2" t="s">
         <v>9</v>
@@ -5235,10 +5236,10 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
+        <v>319</v>
+      </c>
+      <c r="B156" t="s">
         <v>320</v>
-      </c>
-      <c r="B156" t="s">
-        <v>321</v>
       </c>
       <c r="C156" s="2" t="s">
         <v>9</v>
@@ -5258,10 +5259,10 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
+        <v>321</v>
+      </c>
+      <c r="B157" t="s">
         <v>322</v>
-      </c>
-      <c r="B157" t="s">
-        <v>323</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>9</v>
@@ -5281,10 +5282,10 @@
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
+        <v>323</v>
+      </c>
+      <c r="B158" t="s">
         <v>324</v>
-      </c>
-      <c r="B158" t="s">
-        <v>325</v>
       </c>
       <c r="C158" s="2" t="s">
         <v>9</v>
@@ -5304,36 +5305,36 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
+        <v>325</v>
+      </c>
+      <c r="B159" t="s">
         <v>326</v>
       </c>
-      <c r="B159" t="s">
+      <c r="C159" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D159" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E159" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F159" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G159" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H159" t="s">
         <v>327</v>
-      </c>
-      <c r="C159" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D159" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E159" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F159" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G159" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H159" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
+        <v>328</v>
+      </c>
+      <c r="B160" t="s">
         <v>329</v>
-      </c>
-      <c r="B160" t="s">
-        <v>330</v>
       </c>
       <c r="C160" s="4" t="s">
         <v>17</v>
@@ -5353,10 +5354,10 @@
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
+        <v>330</v>
+      </c>
+      <c r="B161" t="s">
         <v>331</v>
-      </c>
-      <c r="B161" t="s">
-        <v>332</v>
       </c>
       <c r="C161" s="2" t="s">
         <v>9</v>
@@ -5376,10 +5377,10 @@
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
+        <v>332</v>
+      </c>
+      <c r="B162" t="s">
         <v>333</v>
-      </c>
-      <c r="B162" t="s">
-        <v>334</v>
       </c>
       <c r="C162" s="2" t="s">
         <v>9</v>
@@ -5399,10 +5400,10 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
+        <v>334</v>
+      </c>
+      <c r="B163" t="s">
         <v>335</v>
-      </c>
-      <c r="B163" t="s">
-        <v>336</v>
       </c>
       <c r="C163" s="4" t="s">
         <v>17</v>
@@ -5422,10 +5423,10 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
+        <v>336</v>
+      </c>
+      <c r="B164" t="s">
         <v>337</v>
-      </c>
-      <c r="B164" t="s">
-        <v>338</v>
       </c>
       <c r="C164" s="4" t="s">
         <v>17</v>
@@ -5445,10 +5446,10 @@
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
+        <v>338</v>
+      </c>
+      <c r="B165" t="s">
         <v>339</v>
-      </c>
-      <c r="B165" t="s">
-        <v>340</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>9</v>
@@ -5468,10 +5469,10 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
+        <v>340</v>
+      </c>
+      <c r="B166" t="s">
         <v>341</v>
-      </c>
-      <c r="B166" t="s">
-        <v>342</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>9</v>
@@ -5491,36 +5492,36 @@
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
+        <v>342</v>
+      </c>
+      <c r="B167" t="s">
         <v>343</v>
       </c>
-      <c r="B167" t="s">
+      <c r="C167" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F167" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G167" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H167" t="s">
         <v>344</v>
-      </c>
-      <c r="C167" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D167" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E167" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F167" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G167" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H167" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
+        <v>345</v>
+      </c>
+      <c r="B168" t="s">
         <v>346</v>
-      </c>
-      <c r="B168" t="s">
-        <v>347</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>9</v>
@@ -5540,10 +5541,10 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
+        <v>347</v>
+      </c>
+      <c r="B169" t="s">
         <v>348</v>
-      </c>
-      <c r="B169" t="s">
-        <v>349</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>9</v>
@@ -5563,10 +5564,10 @@
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
+        <v>349</v>
+      </c>
+      <c r="B170" t="s">
         <v>350</v>
-      </c>
-      <c r="B170" t="s">
-        <v>351</v>
       </c>
       <c r="C170" s="4" t="s">
         <v>17</v>
@@ -5586,10 +5587,10 @@
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
+        <v>351</v>
+      </c>
+      <c r="B171" t="s">
         <v>352</v>
-      </c>
-      <c r="B171" t="s">
-        <v>353</v>
       </c>
       <c r="C171" s="4" t="s">
         <v>17</v>
@@ -5609,10 +5610,10 @@
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
+        <v>353</v>
+      </c>
+      <c r="B172" t="s">
         <v>354</v>
-      </c>
-      <c r="B172" t="s">
-        <v>355</v>
       </c>
       <c r="C172" s="4" t="s">
         <v>17</v>
@@ -5632,10 +5633,10 @@
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
+        <v>355</v>
+      </c>
+      <c r="B173" t="s">
         <v>356</v>
-      </c>
-      <c r="B173" t="s">
-        <v>357</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>9</v>
@@ -5655,10 +5656,10 @@
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
+        <v>357</v>
+      </c>
+      <c r="B174" t="s">
         <v>358</v>
-      </c>
-      <c r="B174" t="s">
-        <v>359</v>
       </c>
       <c r="C174" s="4" t="s">
         <v>17</v>
@@ -5678,10 +5679,10 @@
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
+        <v>359</v>
+      </c>
+      <c r="B175" t="s">
         <v>360</v>
-      </c>
-      <c r="B175" t="s">
-        <v>361</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>9</v>
@@ -5701,10 +5702,10 @@
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
+        <v>361</v>
+      </c>
+      <c r="B176" t="s">
         <v>362</v>
-      </c>
-      <c r="B176" t="s">
-        <v>363</v>
       </c>
       <c r="C176" s="2" t="s">
         <v>9</v>
@@ -5724,10 +5725,10 @@
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
+        <v>363</v>
+      </c>
+      <c r="B177" t="s">
         <v>364</v>
-      </c>
-      <c r="B177" t="s">
-        <v>365</v>
       </c>
       <c r="C177" s="2" t="s">
         <v>9</v>
@@ -5747,10 +5748,10 @@
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
+        <v>365</v>
+      </c>
+      <c r="B178" t="s">
         <v>366</v>
-      </c>
-      <c r="B178" t="s">
-        <v>367</v>
       </c>
       <c r="C178" s="2" t="s">
         <v>9</v>
@@ -5770,10 +5771,10 @@
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
+        <v>367</v>
+      </c>
+      <c r="B179" t="s">
         <v>368</v>
-      </c>
-      <c r="B179" t="s">
-        <v>369</v>
       </c>
       <c r="C179" s="2" t="s">
         <v>9</v>
@@ -5793,10 +5794,10 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
+        <v>369</v>
+      </c>
+      <c r="B180" t="s">
         <v>370</v>
-      </c>
-      <c r="B180" t="s">
-        <v>371</v>
       </c>
       <c r="C180" s="2" t="s">
         <v>9</v>
@@ -5816,10 +5817,10 @@
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
+        <v>371</v>
+      </c>
+      <c r="B181" t="s">
         <v>372</v>
-      </c>
-      <c r="B181" t="s">
-        <v>373</v>
       </c>
       <c r="C181" s="2" t="s">
         <v>9</v>
@@ -5839,10 +5840,10 @@
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
+        <v>373</v>
+      </c>
+      <c r="B182" t="s">
         <v>374</v>
-      </c>
-      <c r="B182" t="s">
-        <v>375</v>
       </c>
       <c r="C182" s="2" t="s">
         <v>9</v>
@@ -5862,10 +5863,10 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
+        <v>375</v>
+      </c>
+      <c r="B183" t="s">
         <v>376</v>
-      </c>
-      <c r="B183" t="s">
-        <v>377</v>
       </c>
       <c r="C183" s="4" t="s">
         <v>17</v>
@@ -5885,10 +5886,10 @@
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
+        <v>377</v>
+      </c>
+      <c r="B184" t="s">
         <v>378</v>
-      </c>
-      <c r="B184" t="s">
-        <v>379</v>
       </c>
       <c r="C184" s="2" t="s">
         <v>9</v>
@@ -5908,10 +5909,10 @@
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
+        <v>379</v>
+      </c>
+      <c r="B185" t="s">
         <v>380</v>
-      </c>
-      <c r="B185" t="s">
-        <v>381</v>
       </c>
       <c r="C185" s="4" t="s">
         <v>17</v>
@@ -5931,10 +5932,10 @@
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
+        <v>381</v>
+      </c>
+      <c r="B186" t="s">
         <v>382</v>
-      </c>
-      <c r="B186" t="s">
-        <v>383</v>
       </c>
       <c r="C186" s="2" t="s">
         <v>9</v>
@@ -5954,10 +5955,10 @@
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
+        <v>383</v>
+      </c>
+      <c r="B187" t="s">
         <v>384</v>
-      </c>
-      <c r="B187" t="s">
-        <v>385</v>
       </c>
       <c r="C187" s="2" t="s">
         <v>9</v>
@@ -5977,10 +5978,10 @@
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
+        <v>385</v>
+      </c>
+      <c r="B188" t="s">
         <v>386</v>
-      </c>
-      <c r="B188" t="s">
-        <v>387</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>9</v>
@@ -6000,10 +6001,10 @@
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
+        <v>387</v>
+      </c>
+      <c r="B189" t="s">
         <v>388</v>
-      </c>
-      <c r="B189" t="s">
-        <v>389</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>9</v>
@@ -6023,10 +6024,10 @@
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
+        <v>389</v>
+      </c>
+      <c r="B190" t="s">
         <v>390</v>
-      </c>
-      <c r="B190" t="s">
-        <v>391</v>
       </c>
       <c r="C190" t="s">
         <v>24</v>
@@ -6046,10 +6047,10 @@
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
+        <v>391</v>
+      </c>
+      <c r="B191" t="s">
         <v>392</v>
-      </c>
-      <c r="B191" t="s">
-        <v>393</v>
       </c>
       <c r="C191" s="4" t="s">
         <v>17</v>
@@ -6069,10 +6070,10 @@
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
+        <v>393</v>
+      </c>
+      <c r="B192" t="s">
         <v>394</v>
-      </c>
-      <c r="B192" t="s">
-        <v>395</v>
       </c>
       <c r="C192" s="2" t="s">
         <v>9</v>
@@ -6092,10 +6093,10 @@
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
+        <v>395</v>
+      </c>
+      <c r="B193" t="s">
         <v>396</v>
-      </c>
-      <c r="B193" t="s">
-        <v>397</v>
       </c>
       <c r="C193" s="4" t="s">
         <v>17</v>
@@ -6115,10 +6116,10 @@
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
+        <v>397</v>
+      </c>
+      <c r="B194" t="s">
         <v>398</v>
-      </c>
-      <c r="B194" t="s">
-        <v>399</v>
       </c>
       <c r="C194" s="4" t="s">
         <v>17</v>
@@ -6138,10 +6139,10 @@
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
+        <v>399</v>
+      </c>
+      <c r="B195" t="s">
         <v>400</v>
-      </c>
-      <c r="B195" t="s">
-        <v>401</v>
       </c>
       <c r="C195" s="2" t="s">
         <v>9</v>
@@ -6161,10 +6162,10 @@
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
+        <v>401</v>
+      </c>
+      <c r="B196" t="s">
         <v>402</v>
-      </c>
-      <c r="B196" t="s">
-        <v>403</v>
       </c>
       <c r="C196" s="4" t="s">
         <v>17</v>
@@ -6184,10 +6185,10 @@
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
+        <v>403</v>
+      </c>
+      <c r="B197" t="s">
         <v>404</v>
-      </c>
-      <c r="B197" t="s">
-        <v>405</v>
       </c>
       <c r="C197" s="2" t="s">
         <v>9</v>
@@ -6207,10 +6208,10 @@
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
+        <v>405</v>
+      </c>
+      <c r="B198" t="s">
         <v>406</v>
-      </c>
-      <c r="B198" t="s">
-        <v>407</v>
       </c>
       <c r="C198" s="2" t="s">
         <v>9</v>
@@ -6230,10 +6231,10 @@
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
+        <v>407</v>
+      </c>
+      <c r="B199" t="s">
         <v>408</v>
-      </c>
-      <c r="B199" t="s">
-        <v>409</v>
       </c>
       <c r="C199" s="2" t="s">
         <v>9</v>
@@ -6253,10 +6254,10 @@
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
+        <v>409</v>
+      </c>
+      <c r="B200" t="s">
         <v>410</v>
-      </c>
-      <c r="B200" t="s">
-        <v>411</v>
       </c>
       <c r="C200" s="2" t="s">
         <v>9</v>
@@ -6276,36 +6277,36 @@
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
+        <v>411</v>
+      </c>
+      <c r="B201" t="s">
         <v>412</v>
       </c>
-      <c r="B201" t="s">
+      <c r="C201" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D201" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E201" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F201" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G201" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H201" t="s">
         <v>413</v>
-      </c>
-      <c r="C201" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D201" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E201" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F201" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G201" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H201" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
+        <v>414</v>
+      </c>
+      <c r="B202" t="s">
         <v>415</v>
-      </c>
-      <c r="B202" t="s">
-        <v>416</v>
       </c>
       <c r="C202" s="2" t="s">
         <v>9</v>
@@ -6325,10 +6326,10 @@
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
+        <v>416</v>
+      </c>
+      <c r="B203" t="s">
         <v>417</v>
-      </c>
-      <c r="B203" t="s">
-        <v>418</v>
       </c>
       <c r="C203" s="2" t="s">
         <v>9</v>

</xml_diff>